<commit_message>
Added computation times comparison.
</commit_message>
<xml_diff>
--- a/comp_time.xlsx
+++ b/comp_time.xlsx
@@ -66,6 +66,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,10 +140,10 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.75"/>
@@ -218,6 +219,9 @@
       <c r="A7" s="0" t="n">
         <v>160</v>
       </c>
+      <c r="B7" s="0" t="n">
+        <v>15.8</v>
+      </c>
       <c r="C7" s="0" t="n">
         <v>0.73</v>
       </c>
@@ -226,6 +230,9 @@
       <c r="A8" s="0" t="n">
         <f aca="false">160*2</f>
         <v>320</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>29.3</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1.45</v>

</xml_diff>